<commit_message>
Added migration and theme code. Needs sorting out, though.
</commit_message>
<xml_diff>
--- a/Notes/sprint.xlsx
+++ b/Notes/sprint.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="we 27-2-15" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -873,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,4 +953,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>